<commit_message>
add: fill metrics from the left corner
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -16,33 +16,36 @@
     <definedName name="activity_month">'Raw_One'!$B$1:$B$1</definedName>
     <definedName name="activity_quarter">'Raw_One'!$C$1:$C$1</definedName>
     <definedName name="activity_year">'Raw_One'!$D$1:$D$1</definedName>
-    <definedName name="seller_origin">'Raw_One'!$E$1:$E$1</definedName>
-    <definedName name="seller_origin_level1">'Raw_One'!$F$1:$F$1</definedName>
-    <definedName name="seller_origin_level2">'Raw_One'!$G$1:$G$1</definedName>
-    <definedName name="wtd_threep_net_ord_gms">'Raw_One'!$H$1:$H$1</definedName>
-    <definedName name="wtd_fba_net_ord_gms">'Raw_One'!$I$1:$I$1</definedName>
-    <definedName name="wtd_mfn_net_ord_gms">'Raw_One'!$J$1:$J$1</definedName>
-    <definedName name="wtd_threep_net_ord_units">'Raw_One'!$K$1:$K$1</definedName>
-    <definedName name="wtd_fba_net_ord_units">'Raw_One'!$L$1:$L$1</definedName>
-    <definedName name="wtd_mfn_net_ord_units">'Raw_One'!$M$1:$M$1</definedName>
-    <definedName name="mtd_threep_net_ord_gms">'Raw_One'!$N$1:$N$1</definedName>
-    <definedName name="mtd_fba_net_ord_gms">'Raw_One'!$O$1:$O$1</definedName>
-    <definedName name="mtd_mfn_net_ord_gms">'Raw_One'!$P$1:$P$1</definedName>
-    <definedName name="mtd_threep_net_ord_units">'Raw_One'!$Q$1:$Q$1</definedName>
-    <definedName name="mtd_fba_net_ord_units">'Raw_One'!$R$1:$R$1</definedName>
-    <definedName name="mtd_mfn_net_ord_units">'Raw_One'!$S$1:$S$1</definedName>
-    <definedName name="qtd_threep_net_ord_gms">'Raw_One'!$T$1:$T$1</definedName>
-    <definedName name="qtd_fba_net_ord_gms">'Raw_One'!$U$1:$U$1</definedName>
-    <definedName name="qtd_mfn_net_ord_gms">'Raw_One'!$V$1:$V$1</definedName>
-    <definedName name="qtd_threep_net_ord_units">'Raw_One'!$W$1:$W$1</definedName>
-    <definedName name="qtd_fba_net_ord_units">'Raw_One'!$X$1:$X$1</definedName>
-    <definedName name="qtd_mfn_net_ord_units">'Raw_One'!$Y$1:$Y$1</definedName>
-    <definedName name="ytd_threep_net_ord_gms">'Raw_One'!$Z$1:$Z$1</definedName>
-    <definedName name="ytd_fba_net_ord_gms">'Raw_One'!$AA$1:$AA$1</definedName>
-    <definedName name="ytd_mfn_net_ord_gms">'Raw_One'!$AB$1:$AB$1</definedName>
-    <definedName name="ytd_threep_net_ord_units">'Raw_One'!$AC$1:$AC$1</definedName>
-    <definedName name="ytd_fba_net_ord_units">'Raw_One'!$AD$1:$AD$1</definedName>
-    <definedName name="ytd_mfn_net_ord_units">'Raw_One'!$AE$1:$AE$1</definedName>
+    <definedName name="region">'Raw_One'!$E$1:$E$1</definedName>
+    <definedName name="marketplace_id">'Raw_One'!$F$1:$F$1</definedName>
+    <definedName name="marketplace_name">'Raw_One'!$G$1:$G$1</definedName>
+    <definedName name="seller_origin">'Raw_One'!$H$1:$H$1</definedName>
+    <definedName name="seller_origin_level1">'Raw_One'!$I$1:$I$1</definedName>
+    <definedName name="seller_origin_level2">'Raw_One'!$J$1:$J$1</definedName>
+    <definedName name="wtd_threep_net_ord_gms">'Raw_One'!$K$1:$K$1</definedName>
+    <definedName name="wtd_fba_net_ord_gms">'Raw_One'!$L$1:$L$1</definedName>
+    <definedName name="wtd_mfn_net_ord_gms">'Raw_One'!$M$1:$M$1</definedName>
+    <definedName name="wtd_threep_net_ord_units">'Raw_One'!$N$1:$N$1</definedName>
+    <definedName name="wtd_fba_net_ord_units">'Raw_One'!$O$1:$O$1</definedName>
+    <definedName name="wtd_mfn_net_ord_units">'Raw_One'!$P$1:$P$1</definedName>
+    <definedName name="mtd_threep_net_ord_gms">'Raw_One'!$Q$1:$Q$1</definedName>
+    <definedName name="mtd_fba_net_ord_gms">'Raw_One'!$R$1:$R$1</definedName>
+    <definedName name="mtd_mfn_net_ord_gms">'Raw_One'!$S$1:$S$1</definedName>
+    <definedName name="mtd_threep_net_ord_units">'Raw_One'!$T$1:$T$1</definedName>
+    <definedName name="mtd_fba_net_ord_units">'Raw_One'!$U$1:$U$1</definedName>
+    <definedName name="mtd_mfn_net_ord_units">'Raw_One'!$V$1:$V$1</definedName>
+    <definedName name="qtd_threep_net_ord_gms">'Raw_One'!$W$1:$W$1</definedName>
+    <definedName name="qtd_fba_net_ord_gms">'Raw_One'!$X$1:$X$1</definedName>
+    <definedName name="qtd_mfn_net_ord_gms">'Raw_One'!$Y$1:$Y$1</definedName>
+    <definedName name="qtd_threep_net_ord_units">'Raw_One'!$Z$1:$Z$1</definedName>
+    <definedName name="qtd_fba_net_ord_units">'Raw_One'!$AA$1:$AA$1</definedName>
+    <definedName name="qtd_mfn_net_ord_units">'Raw_One'!$AB$1:$AB$1</definedName>
+    <definedName name="ytd_threep_net_ord_gms">'Raw_One'!$AC$1:$AC$1</definedName>
+    <definedName name="ytd_fba_net_ord_gms">'Raw_One'!$AD$1:$AD$1</definedName>
+    <definedName name="ytd_mfn_net_ord_gms">'Raw_One'!$AE$1:$AE$1</definedName>
+    <definedName name="ytd_threep_net_ord_units">'Raw_One'!$AF$1:$AF$1</definedName>
+    <definedName name="ytd_fba_net_ord_units">'Raw_One'!$AG$1:$AG$1</definedName>
+    <definedName name="ytd_mfn_net_ord_units">'Raw_One'!$AH$1:$AH$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -595,289 +598,865 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>fba_net_ord_gms</t>
+          <t>wtd_fba_net_ord_gms</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
+      </c>
+      <c r="J12">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="K12">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="L12">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="M12">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="N12">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="O12">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <v/>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>fba_net_ord_gms</t>
+          <t>wtd_fba_net_ord_gms</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>EU</t>
         </is>
+      </c>
+      <c r="J13">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="K13">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="L13">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="M13">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="N13">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="O13">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>fba_net_ord_gms</t>
+          <t>wtd_fba_net_ord_gms</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>JP</t>
         </is>
+      </c>
+      <c r="J14">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="K14">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="L14">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="M14">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="N14">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="O14">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>fba_net_ord_gms</t>
+          <t>wtd_fba_net_ord_gms</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>Emerging</t>
         </is>
+      </c>
+      <c r="J15">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,J4,activity_week,J3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="K15">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,K4,activity_week,K3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="L15">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,L4,activity_week,L3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="M15">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,M4,activity_week,M3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="N15">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,N4,activity_week,N3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="O15">
+        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>fba_net_ord_units</t>
+          <t>wtd_fba_net_ord_units</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
+      </c>
+      <c r="J16">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="K16">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="L16">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="M16">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="N16">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="O16">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>fba_net_ord_units</t>
+          <t>wtd_fba_net_ord_units</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>EU</t>
         </is>
+      </c>
+      <c r="J17">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="K17">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="L17">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="M17">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="N17">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="O17">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <v/>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>fba_net_ord_units</t>
+          <t>wtd_fba_net_ord_units</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>JP</t>
         </is>
+      </c>
+      <c r="J18">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="K18">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="L18">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="M18">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="N18">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="O18">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>fba_net_ord_units</t>
+          <t>wtd_fba_net_ord_units</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>Emerging</t>
         </is>
+      </c>
+      <c r="J19">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,J4,activity_week,J3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="K19">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,K4,activity_week,K3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="L19">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,L4,activity_week,L3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="M19">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,M4,activity_week,M3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="N19">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,N4,activity_week,N3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="O19">
+        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+        <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>mfn_net_ord_gms</t>
+          <t>wtd_mfn_net_ord_gms</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
+      </c>
+      <c r="J20">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="K20">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="L20">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="M20">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="N20">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="O20">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>mfn_net_ord_gms</t>
+          <t>wtd_mfn_net_ord_gms</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>EU</t>
         </is>
+      </c>
+      <c r="J21">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="K21">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="L21">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="M21">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="N21">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="O21">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>mfn_net_ord_gms</t>
+          <t>wtd_mfn_net_ord_gms</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>JP</t>
         </is>
+      </c>
+      <c r="J22">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="K22">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="L22">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="M22">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="N22">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="O22">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>mfn_net_ord_gms</t>
+          <t>wtd_mfn_net_ord_gms</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>Emerging</t>
         </is>
+      </c>
+      <c r="J23">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,J4,activity_week,J3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="K23">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,K4,activity_week,K3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="L23">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,L4,activity_week,L3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="M23">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,M4,activity_week,M3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="N23">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,N4,activity_week,N3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="O23">
+        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+        <v/>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>mfn_net_ord_units</t>
+          <t>wtd_mfn_net_ord_units</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
+      </c>
+      <c r="J24">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="K24">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="L24">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="M24">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="N24">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="O24">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>mfn_net_ord_units</t>
+          <t>wtd_mfn_net_ord_units</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
           <t>EU</t>
         </is>
+      </c>
+      <c r="J25">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="K25">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="L25">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="M25">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="N25">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="O25">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>mfn_net_ord_units</t>
+          <t>wtd_mfn_net_ord_units</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>JP</t>
         </is>
+      </c>
+      <c r="J26">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="K26">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="L26">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="M26">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="N26">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="O26">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>mfn_net_ord_units</t>
+          <t>wtd_mfn_net_ord_units</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
           <t>Emerging</t>
         </is>
+      </c>
+      <c r="J27">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,J4,activity_week,J3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="K27">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,K4,activity_week,K3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="L27">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,L4,activity_week,L3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="M27">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,M4,activity_week,M3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="N27">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,N4,activity_week,N3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="O27">
+        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+        <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>net_ord_gms</t>
+          <t>wtd_net_ord_gms</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
+      </c>
+      <c r="J28">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="K28">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="L28">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="M28">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="N28">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="O28">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>net_ord_gms</t>
+          <t>wtd_net_ord_gms</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>EU</t>
         </is>
+      </c>
+      <c r="J29">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="K29">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="L29">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="M29">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="N29">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="O29">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <v/>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>net_ord_gms</t>
+          <t>wtd_net_ord_gms</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
           <t>JP</t>
         </is>
+      </c>
+      <c r="J30">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="K30">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="L30">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="M30">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="N30">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="O30">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>net_ord_gms</t>
+          <t>wtd_net_ord_gms</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>Emerging</t>
         </is>
+      </c>
+      <c r="J31">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,J4,activity_week,J3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="K31">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,K4,activity_week,K3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="L31">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,L4,activity_week,L3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="M31">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,M4,activity_week,M3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="N31">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,N4,activity_week,N3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="O31">
+        <f>SUMIFS(wtd_net_ord_gms,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+        <v/>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>net_ord_units</t>
+          <t>wtd_net_ord_units</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
+      </c>
+      <c r="J32">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="K32">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="L32">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="M32">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="N32">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <v/>
+      </c>
+      <c r="O32">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <v/>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>net_ord_units</t>
+          <t>wtd_net_ord_units</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
           <t>EU</t>
         </is>
+      </c>
+      <c r="J33">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="K33">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="L33">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="M33">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="N33">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <v/>
+      </c>
+      <c r="O33">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <v/>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>net_ord_units</t>
+          <t>wtd_net_ord_units</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
           <t>JP</t>
         </is>
+      </c>
+      <c r="J34">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="K34">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="L34">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="M34">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="N34">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <v/>
+      </c>
+      <c r="O34">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <v/>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>net_ord_units</t>
+          <t>wtd_net_ord_units</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
           <t>Emerging</t>
         </is>
+      </c>
+      <c r="J35">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,J4,activity_week,J3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="K35">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,K4,activity_week,K3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="L35">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,L4,activity_week,L3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="M35">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,M4,activity_week,M3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="N35">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,N4,activity_week,N3,region,"Emerging")</f>
+        <v/>
+      </c>
+      <c r="O35">
+        <f>SUMIFS(wtd_net_ord_units,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -956,7 +1535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -987,135 +1566,150 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>region</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>marketplace_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>marketplace_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>seller_origin</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>seller_origin_level1</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>seller_origin_level2</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>wtd_threep_net_ord_gms</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>wtd_fba_net_ord_gms</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>wtd_mfn_net_ord_gms</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>wtd_threep_net_ord_units</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>wtd_fba_net_ord_units</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>wtd_mfn_net_ord_units</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>mtd_threep_net_ord_gms</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>mtd_fba_net_ord_gms</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>mtd_mfn_net_ord_gms</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>mtd_threep_net_ord_units</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>mtd_fba_net_ord_units</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>mtd_mfn_net_ord_units</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>qtd_threep_net_ord_gms</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>qtd_fba_net_ord_gms</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>qtd_mfn_net_ord_gms</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>qtd_threep_net_ord_units</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>qtd_fba_net_ord_units</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>qtd_mfn_net_ord_units</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>ytd_threep_net_ord_gms</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>ytd_fba_net_ord_gms</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>ytd_mfn_net_ord_gms</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>ytd_threep_net_ord_units</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>ytd_fba_net_ord_units</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>ytd_mfn_net_ord_units</t>
         </is>

</xml_diff>

<commit_message>
test version for generating excel
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -53,8 +53,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -62,16 +64,46 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <sz val="14"/>
+    </font>
+    <font/>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
+        <bgColor rgb="00D3D3D3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -79,15 +111,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="standardise_date" xfId="1" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -450,7 +498,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,60 +507,72 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="J1" t="n">
-        <v>-35</v>
-      </c>
-      <c r="K1" t="n">
-        <v>-28</v>
-      </c>
-      <c r="L1" t="n">
-        <v>-21</v>
-      </c>
-      <c r="M1" t="n">
-        <v>-14</v>
-      </c>
-      <c r="N1" t="n">
-        <v>-7</v>
-      </c>
-      <c r="O1" t="n">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>REPORTING NAME HERE</t>
+        </is>
+      </c>
+      <c r="P1" t="n">
+        <v>-4</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="R1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="S1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-10-14</t>
-        </is>
-      </c>
-      <c r="J2">
-        <f>A2+J1</f>
-        <v/>
-      </c>
-      <c r="K2">
-        <f>A2+K1</f>
-        <v/>
-      </c>
-      <c r="L2">
-        <f>A2+L1</f>
-        <v/>
-      </c>
-      <c r="M2">
-        <f>A2+M1</f>
-        <v/>
-      </c>
-      <c r="N2">
-        <f>A2+N1</f>
-        <v/>
-      </c>
-      <c r="O2">
-        <f>A2+O1</f>
+      <c r="A2">
+        <f>'_METADATA_'!B1</f>
+        <v/>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="n"/>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1">
+        <f>_xlfn.EOMONTH(A2,                    P1)</f>
+        <v/>
+      </c>
+      <c r="Q2" s="1">
+        <f>_xlfn.EOMONTH(A2,                    Q1)</f>
+        <v/>
+      </c>
+      <c r="R2" s="1">
+        <f>_xlfn.EOMONTH(A2,                    R1)</f>
+        <v/>
+      </c>
+      <c r="S2" s="1">
+        <f>_xlfn.EOMONTH(A2,                    S1)</f>
+        <v/>
+      </c>
+      <c r="T2" s="1">
+        <f>_xlfn.EOMONTH(A2,                    T1)</f>
         <v/>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>VN</t>
+      <c r="A3">
+        <f>'_METADATA_'!B3</f>
+        <v/>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>activity_week</t>
         </is>
       </c>
       <c r="J3">
@@ -541,64 +601,281 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>12345</v>
+      <c r="A4">
+        <f>'_METADATA_'!B4</f>
+        <v/>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>activity_month</t>
+        </is>
       </c>
       <c r="J4">
+        <f>_xlfn.MONTH(J2)</f>
+        <v/>
+      </c>
+      <c r="K4">
+        <f>_xlfn.MONTH(K2)</f>
+        <v/>
+      </c>
+      <c r="L4">
+        <f>_xlfn.MONTH(L2)</f>
+        <v/>
+      </c>
+      <c r="M4">
+        <f>_xlfn.MONTH(M2)</f>
+        <v/>
+      </c>
+      <c r="N4">
+        <f>_xlfn.MONTH(N2)</f>
+        <v/>
+      </c>
+      <c r="O4">
+        <f>_xlfn.MONTH(O2)</f>
+        <v/>
+      </c>
+      <c r="P4">
+        <f>_xlfn.MONTH(P2)</f>
+        <v/>
+      </c>
+      <c r="Q4">
+        <f>_xlfn.MONTH(Q2)</f>
+        <v/>
+      </c>
+      <c r="R4">
+        <f>_xlfn.MONTH(R2)</f>
+        <v/>
+      </c>
+      <c r="S4">
+        <f>_xlfn.MONTH(S2)</f>
+        <v/>
+      </c>
+      <c r="T4">
+        <f>_xlfn.MONTH(T2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>activity_quarter</t>
+        </is>
+      </c>
+      <c r="J5">
+        <f>_xlfn.ROUNDUP(J4/3,0)</f>
+        <v/>
+      </c>
+      <c r="K5">
+        <f>_xlfn.ROUNDUP(K4/3,0)</f>
+        <v/>
+      </c>
+      <c r="L5">
+        <f>_xlfn.ROUNDUP(L4/3,0)</f>
+        <v/>
+      </c>
+      <c r="M5">
+        <f>_xlfn.ROUNDUP(M4/3,0)</f>
+        <v/>
+      </c>
+      <c r="N5">
+        <f>_xlfn.ROUNDUP(N4/3,0)</f>
+        <v/>
+      </c>
+      <c r="O5">
+        <f>_xlfn.ROUNDUP(O4/3,0)</f>
+        <v/>
+      </c>
+      <c r="P5">
+        <f>_xlfn.ROUNDUP(P4/3,0)</f>
+        <v/>
+      </c>
+      <c r="Q5">
+        <f>_xlfn.ROUNDUP(Q4/3,0)</f>
+        <v/>
+      </c>
+      <c r="R5">
+        <f>_xlfn.ROUNDUP(R4/3,0)</f>
+        <v/>
+      </c>
+      <c r="S5">
+        <f>_xlfn.ROUNDUP(S4/3,0)</f>
+        <v/>
+      </c>
+      <c r="T5">
+        <f>_xlfn.ROUNDUP(T4/3,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>activity_year</t>
+        </is>
+      </c>
+      <c r="J6">
         <f>YEAR(J2)</f>
         <v/>
       </c>
-      <c r="K4">
+      <c r="K6">
         <f>YEAR(K2)</f>
         <v/>
       </c>
-      <c r="L4">
+      <c r="L6">
         <f>YEAR(L2)</f>
         <v/>
       </c>
-      <c r="M4">
+      <c r="M6">
         <f>YEAR(M2)</f>
         <v/>
       </c>
-      <c r="N4">
+      <c r="N6">
         <f>YEAR(N2)</f>
         <v/>
       </c>
-      <c r="O4">
+      <c r="O6">
         <f>YEAR(O2)</f>
         <v/>
       </c>
+      <c r="P6">
+        <f>YEAR(P2)</f>
+        <v/>
+      </c>
+      <c r="Q6">
+        <f>YEAR(Q2)</f>
+        <v/>
+      </c>
+      <c r="R6">
+        <f>YEAR(R2)</f>
+        <v/>
+      </c>
+      <c r="S6">
+        <f>YEAR(S2)</f>
+        <v/>
+      </c>
+      <c r="T6">
+        <f>YEAR(T2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>REPORTING NAME HERE</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="J10">
-        <f>"Wk"&amp;J3&amp;"-"&amp;RIGHT(J4,2)</f>
-        <v/>
-      </c>
-      <c r="K10">
-        <f>"Wk"&amp;K3&amp;"-"&amp;RIGHT(K4,2)</f>
-        <v/>
-      </c>
-      <c r="L10">
-        <f>"Wk"&amp;L3&amp;"-"&amp;RIGHT(L4,2)</f>
-        <v/>
-      </c>
-      <c r="M10">
-        <f>"Wk"&amp;M3&amp;"-"&amp;RIGHT(M4,2)</f>
-        <v/>
-      </c>
-      <c r="N10">
-        <f>"Wk"&amp;N3&amp;"-"&amp;RIGHT(N4,2)</f>
-        <v/>
-      </c>
-      <c r="O10">
-        <f>"Wk"&amp;O3&amp;"-"&amp;RIGHT(O4,2)</f>
+      <c r="I10" s="3" t="n"/>
+      <c r="J10" s="4">
+        <f>"Wk"&amp;J3                    &amp;"-"&amp;                    RIGHT(J6,2)</f>
+        <v/>
+      </c>
+      <c r="K10" s="4">
+        <f>"Wk"&amp;K3                    &amp;"-"&amp;                    RIGHT(K6,2)</f>
+        <v/>
+      </c>
+      <c r="L10" s="4">
+        <f>"Wk"&amp;L3                    &amp;"-"&amp;                    RIGHT(L6,2)</f>
+        <v/>
+      </c>
+      <c r="M10" s="4">
+        <f>"Wk"&amp;M3                    &amp;"-"&amp;                    RIGHT(M6,2)</f>
+        <v/>
+      </c>
+      <c r="N10" s="4">
+        <f>"Wk"&amp;N3                    &amp;"-"&amp;                    RIGHT(N6,2)</f>
+        <v/>
+      </c>
+      <c r="O10" s="4">
+        <f>"Wk"&amp;O3                    &amp;"-"&amp;                    RIGHT(O6,2)</f>
+        <v/>
+      </c>
+      <c r="P10" s="4">
+        <f>TEXT(P4*28, "mmm")                    &amp;"-"&amp;RIGHT(P6,2)</f>
+        <v/>
+      </c>
+      <c r="Q10" s="4">
+        <f>TEXT(Q4*28, "mmm")                    &amp;"-"&amp;RIGHT(Q6,2)</f>
+        <v/>
+      </c>
+      <c r="R10" s="4">
+        <f>TEXT(R4*28, "mmm")                    &amp;"-"&amp;RIGHT(R6,2)</f>
+        <v/>
+      </c>
+      <c r="S10" s="4">
+        <f>TEXT(S4*28, "mmm")                    &amp;"-"&amp;RIGHT(S6,2)</f>
+        <v/>
+      </c>
+      <c r="T10" s="4">
+        <f>TEXT(T4*28, "mmm")                    &amp;"-"&amp;RIGHT(T6,2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>wtd_threep_net_ord_gms</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AGG</t>
+        </is>
+      </c>
+      <c r="I11" s="5" t="inlineStr">
+        <is>
+          <t>Net Ordered GMS</t>
+        </is>
+      </c>
+      <c r="J11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,J6,                activity_week,J3,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="K11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,K6,                activity_week,K3,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="L11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,L6,                activity_week,L3,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="M11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,M6,                activity_week,M3,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="N11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,N6,                activity_week,N3,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="O11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,O6,                activity_week,O3,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="P11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,P6,                activity_month,P4,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="Q11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,Q6,                activity_month,Q4,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="R11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,R6,                activity_month,R4,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="S11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,S6,                activity_month,S4,                region,$B11)</f>
+        <v/>
+      </c>
+      <c r="T11" s="6">
+        <f>SUMIFS(                INDIRECT($A11),                activity_year,T6,                activity_month,T4,                region,$B11)</f>
         <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>wtd_fba_net_ord_gms</t>
+          <t>wtd_threep_net_ord_gms</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -606,35 +883,60 @@
           <t>NA</t>
         </is>
       </c>
+      <c r="I12" s="7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="J12">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,J6,                activity_week,J3,                region,$B12)</f>
         <v/>
       </c>
       <c r="K12">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,K6,                activity_week,K3,                region,$B12)</f>
         <v/>
       </c>
       <c r="L12">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,L6,                activity_week,L3,                region,$B12)</f>
         <v/>
       </c>
       <c r="M12">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,M6,                activity_week,M3,                region,$B12)</f>
         <v/>
       </c>
       <c r="N12">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,N6,                activity_week,N3,                region,$B12)</f>
         <v/>
       </c>
       <c r="O12">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,O6,                activity_week,O3,                region,$B12)</f>
+        <v/>
+      </c>
+      <c r="P12">
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,P6,                activity_month,P4,                region,$B12)</f>
+        <v/>
+      </c>
+      <c r="Q12">
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,Q6,                activity_month,Q4,                region,$B12)</f>
+        <v/>
+      </c>
+      <c r="R12">
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,R6,                activity_month,R4,                region,$B12)</f>
+        <v/>
+      </c>
+      <c r="S12">
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,S6,                activity_month,S4,                region,$B12)</f>
+        <v/>
+      </c>
+      <c r="T12">
+        <f>SUMIFS(                INDIRECT($A12),                activity_year,T6,                activity_month,T4,                region,$B12)</f>
         <v/>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>wtd_fba_net_ord_gms</t>
+          <t>wtd_threep_net_ord_gms</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -642,35 +944,60 @@
           <t>EU</t>
         </is>
       </c>
+      <c r="I13" s="7" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
       <c r="J13">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,J6,                activity_week,J3,                region,$B13)</f>
         <v/>
       </c>
       <c r="K13">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,K6,                activity_week,K3,                region,$B13)</f>
         <v/>
       </c>
       <c r="L13">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,L6,                activity_week,L3,                region,$B13)</f>
         <v/>
       </c>
       <c r="M13">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,M6,                activity_week,M3,                region,$B13)</f>
         <v/>
       </c>
       <c r="N13">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,N6,                activity_week,N3,                region,$B13)</f>
         <v/>
       </c>
       <c r="O13">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,O6,                activity_week,O3,                region,$B13)</f>
+        <v/>
+      </c>
+      <c r="P13">
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,P6,                activity_month,P4,                region,$B13)</f>
+        <v/>
+      </c>
+      <c r="Q13">
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,Q6,                activity_month,Q4,                region,$B13)</f>
+        <v/>
+      </c>
+      <c r="R13">
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,R6,                activity_month,R4,                region,$B13)</f>
+        <v/>
+      </c>
+      <c r="S13">
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,S6,                activity_month,S4,                region,$B13)</f>
+        <v/>
+      </c>
+      <c r="T13">
+        <f>SUMIFS(                INDIRECT($A13),                activity_year,T6,                activity_month,T4,                region,$B13)</f>
         <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>wtd_fba_net_ord_gms</t>
+          <t>wtd_threep_net_ord_gms</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -678,28 +1005,53 @@
           <t>JP</t>
         </is>
       </c>
+      <c r="I14" s="7" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="J14">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,J6,                activity_week,J3,                region,$B14)</f>
         <v/>
       </c>
       <c r="K14">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,K6,                activity_week,K3,                region,$B14)</f>
         <v/>
       </c>
       <c r="L14">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,L6,                activity_week,L3,                region,$B14)</f>
         <v/>
       </c>
       <c r="M14">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,M6,                activity_week,M3,                region,$B14)</f>
         <v/>
       </c>
       <c r="N14">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,N6,                activity_week,N3,                region,$B14)</f>
         <v/>
       </c>
       <c r="O14">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,O6,                activity_week,O3,                region,$B14)</f>
+        <v/>
+      </c>
+      <c r="P14">
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,P6,                activity_month,P4,                region,$B14)</f>
+        <v/>
+      </c>
+      <c r="Q14">
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,Q6,                activity_month,Q4,                region,$B14)</f>
+        <v/>
+      </c>
+      <c r="R14">
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,R6,                activity_month,R4,                region,$B14)</f>
+        <v/>
+      </c>
+      <c r="S14">
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,S6,                activity_month,S4,                region,$B14)</f>
+        <v/>
+      </c>
+      <c r="T14">
+        <f>SUMIFS(                INDIRECT($A14),                activity_year,T6,                activity_month,T4,                region,$B14)</f>
         <v/>
       </c>
     </row>
@@ -711,38 +1063,63 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Emerging</t>
-        </is>
-      </c>
-      <c r="J15">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,J4,activity_week,J3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="K15">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,K4,activity_week,K3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="L15">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,L4,activity_week,L3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="M15">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,M4,activity_week,M3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="N15">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,N4,activity_week,N3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="O15">
-        <f>SUMIFS(wtd_fba_net_ord_gms,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+          <t>AGG</t>
+        </is>
+      </c>
+      <c r="I15" s="5" t="inlineStr">
+        <is>
+          <t>FBA Net Ordered GMS</t>
+        </is>
+      </c>
+      <c r="J15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,J6,                activity_week,J3,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="K15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,K6,                activity_week,K3,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="L15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,L6,                activity_week,L3,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="M15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,M6,                activity_week,M3,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="N15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,N6,                activity_week,N3,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="O15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,O6,                activity_week,O3,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="P15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,P6,                activity_month,P4,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="Q15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,Q6,                activity_month,Q4,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="R15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,R6,                activity_month,R4,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="S15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,S6,                activity_month,S4,                region,$B15)</f>
+        <v/>
+      </c>
+      <c r="T15" s="6">
+        <f>SUMIFS(                INDIRECT($A15),                activity_year,T6,                activity_month,T4,                region,$B15)</f>
         <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>wtd_fba_net_ord_units</t>
+          <t>wtd_fba_net_ord_gms</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -750,35 +1127,60 @@
           <t>NA</t>
         </is>
       </c>
+      <c r="I16" s="7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="J16">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,J6,                activity_week,J3,                region,$B16)</f>
         <v/>
       </c>
       <c r="K16">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,K6,                activity_week,K3,                region,$B16)</f>
         <v/>
       </c>
       <c r="L16">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,L6,                activity_week,L3,                region,$B16)</f>
         <v/>
       </c>
       <c r="M16">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,M6,                activity_week,M3,                region,$B16)</f>
         <v/>
       </c>
       <c r="N16">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,N6,                activity_week,N3,                region,$B16)</f>
         <v/>
       </c>
       <c r="O16">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,O6,                activity_week,O3,                region,$B16)</f>
+        <v/>
+      </c>
+      <c r="P16">
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,P6,                activity_month,P4,                region,$B16)</f>
+        <v/>
+      </c>
+      <c r="Q16">
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,Q6,                activity_month,Q4,                region,$B16)</f>
+        <v/>
+      </c>
+      <c r="R16">
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,R6,                activity_month,R4,                region,$B16)</f>
+        <v/>
+      </c>
+      <c r="S16">
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,S6,                activity_month,S4,                region,$B16)</f>
+        <v/>
+      </c>
+      <c r="T16">
+        <f>SUMIFS(                INDIRECT($A16),                activity_year,T6,                activity_month,T4,                region,$B16)</f>
         <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>wtd_fba_net_ord_units</t>
+          <t>wtd_fba_net_ord_gms</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -786,35 +1188,60 @@
           <t>EU</t>
         </is>
       </c>
+      <c r="I17" s="7" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
       <c r="J17">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,J6,                activity_week,J3,                region,$B17)</f>
         <v/>
       </c>
       <c r="K17">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,K6,                activity_week,K3,                region,$B17)</f>
         <v/>
       </c>
       <c r="L17">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,L6,                activity_week,L3,                region,$B17)</f>
         <v/>
       </c>
       <c r="M17">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,M6,                activity_week,M3,                region,$B17)</f>
         <v/>
       </c>
       <c r="N17">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,N6,                activity_week,N3,                region,$B17)</f>
         <v/>
       </c>
       <c r="O17">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,O6,                activity_week,O3,                region,$B17)</f>
+        <v/>
+      </c>
+      <c r="P17">
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,P6,                activity_month,P4,                region,$B17)</f>
+        <v/>
+      </c>
+      <c r="Q17">
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,Q6,                activity_month,Q4,                region,$B17)</f>
+        <v/>
+      </c>
+      <c r="R17">
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,R6,                activity_month,R4,                region,$B17)</f>
+        <v/>
+      </c>
+      <c r="S17">
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,S6,                activity_month,S4,                region,$B17)</f>
+        <v/>
+      </c>
+      <c r="T17">
+        <f>SUMIFS(                INDIRECT($A17),                activity_year,T6,                activity_month,T4,                region,$B17)</f>
         <v/>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>wtd_fba_net_ord_units</t>
+          <t>wtd_fba_net_ord_gms</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -822,64 +1249,114 @@
           <t>JP</t>
         </is>
       </c>
+      <c r="I18" s="7" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="J18">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,J6,                activity_week,J3,                region,$B18)</f>
         <v/>
       </c>
       <c r="K18">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,K6,                activity_week,K3,                region,$B18)</f>
         <v/>
       </c>
       <c r="L18">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,L6,                activity_week,L3,                region,$B18)</f>
         <v/>
       </c>
       <c r="M18">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,M6,                activity_week,M3,                region,$B18)</f>
         <v/>
       </c>
       <c r="N18">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,N6,                activity_week,N3,                region,$B18)</f>
         <v/>
       </c>
       <c r="O18">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,O6,                activity_week,O3,                region,$B18)</f>
+        <v/>
+      </c>
+      <c r="P18">
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,P6,                activity_month,P4,                region,$B18)</f>
+        <v/>
+      </c>
+      <c r="Q18">
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,Q6,                activity_month,Q4,                region,$B18)</f>
+        <v/>
+      </c>
+      <c r="R18">
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,R6,                activity_month,R4,                region,$B18)</f>
+        <v/>
+      </c>
+      <c r="S18">
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,S6,                activity_month,S4,                region,$B18)</f>
+        <v/>
+      </c>
+      <c r="T18">
+        <f>SUMIFS(                INDIRECT($A18),                activity_year,T6,                activity_month,T4,                region,$B18)</f>
         <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>wtd_fba_net_ord_units</t>
+          <t>wtd_mfn_net_ord_gms</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Emerging</t>
-        </is>
-      </c>
-      <c r="J19">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,J4,activity_week,J3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="K19">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,K4,activity_week,K3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="L19">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,L4,activity_week,L3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="M19">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,M4,activity_week,M3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="N19">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,N4,activity_week,N3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="O19">
-        <f>SUMIFS(wtd_fba_net_ord_units,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+          <t>AGG</t>
+        </is>
+      </c>
+      <c r="I19" s="5" t="inlineStr">
+        <is>
+          <t>MFN Net Ordered GMS</t>
+        </is>
+      </c>
+      <c r="J19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,J6,                activity_week,J3,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="K19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,K6,                activity_week,K3,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="L19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,L6,                activity_week,L3,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="M19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,M6,                activity_week,M3,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="N19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,N6,                activity_week,N3,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="O19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,O6,                activity_week,O3,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="P19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,P6,                activity_month,P4,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="Q19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,Q6,                activity_month,Q4,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="R19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,R6,                activity_month,R4,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="S19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,S6,                activity_month,S4,                region,$B19)</f>
+        <v/>
+      </c>
+      <c r="T19" s="6">
+        <f>SUMIFS(                INDIRECT($A19),                activity_year,T6,                activity_month,T4,                region,$B19)</f>
         <v/>
       </c>
     </row>
@@ -894,28 +1371,53 @@
           <t>NA</t>
         </is>
       </c>
+      <c r="I20" s="7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="J20">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,J6,                activity_week,J3,                region,$B20)</f>
         <v/>
       </c>
       <c r="K20">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,K6,                activity_week,K3,                region,$B20)</f>
         <v/>
       </c>
       <c r="L20">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,L6,                activity_week,L3,                region,$B20)</f>
         <v/>
       </c>
       <c r="M20">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,M6,                activity_week,M3,                region,$B20)</f>
         <v/>
       </c>
       <c r="N20">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,N6,                activity_week,N3,                region,$B20)</f>
         <v/>
       </c>
       <c r="O20">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,O6,                activity_week,O3,                region,$B20)</f>
+        <v/>
+      </c>
+      <c r="P20">
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,P6,                activity_month,P4,                region,$B20)</f>
+        <v/>
+      </c>
+      <c r="Q20">
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,Q6,                activity_month,Q4,                region,$B20)</f>
+        <v/>
+      </c>
+      <c r="R20">
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,R6,                activity_month,R4,                region,$B20)</f>
+        <v/>
+      </c>
+      <c r="S20">
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,S6,                activity_month,S4,                region,$B20)</f>
+        <v/>
+      </c>
+      <c r="T20">
+        <f>SUMIFS(                INDIRECT($A20),                activity_year,T6,                activity_month,T4,                region,$B20)</f>
         <v/>
       </c>
     </row>
@@ -930,28 +1432,53 @@
           <t>EU</t>
         </is>
       </c>
+      <c r="I21" s="7" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
       <c r="J21">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,J6,                activity_week,J3,                region,$B21)</f>
         <v/>
       </c>
       <c r="K21">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,K6,                activity_week,K3,                region,$B21)</f>
         <v/>
       </c>
       <c r="L21">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,L6,                activity_week,L3,                region,$B21)</f>
         <v/>
       </c>
       <c r="M21">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,M6,                activity_week,M3,                region,$B21)</f>
         <v/>
       </c>
       <c r="N21">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,N6,                activity_week,N3,                region,$B21)</f>
         <v/>
       </c>
       <c r="O21">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,O6,                activity_week,O3,                region,$B21)</f>
+        <v/>
+      </c>
+      <c r="P21">
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,P6,                activity_month,P4,                region,$B21)</f>
+        <v/>
+      </c>
+      <c r="Q21">
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,Q6,                activity_month,Q4,                region,$B21)</f>
+        <v/>
+      </c>
+      <c r="R21">
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,R6,                activity_month,R4,                region,$B21)</f>
+        <v/>
+      </c>
+      <c r="S21">
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,S6,                activity_month,S4,                region,$B21)</f>
+        <v/>
+      </c>
+      <c r="T21">
+        <f>SUMIFS(                INDIRECT($A21),                activity_year,T6,                activity_month,T4,                region,$B21)</f>
         <v/>
       </c>
     </row>
@@ -966,71 +1493,121 @@
           <t>JP</t>
         </is>
       </c>
+      <c r="I22" s="7" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="J22">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,J6,                activity_week,J3,                region,$B22)</f>
         <v/>
       </c>
       <c r="K22">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,K6,                activity_week,K3,                region,$B22)</f>
         <v/>
       </c>
       <c r="L22">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,L6,                activity_week,L3,                region,$B22)</f>
         <v/>
       </c>
       <c r="M22">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,M6,                activity_week,M3,                region,$B22)</f>
         <v/>
       </c>
       <c r="N22">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,N6,                activity_week,N3,                region,$B22)</f>
         <v/>
       </c>
       <c r="O22">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,O6,                activity_week,O3,                region,$B22)</f>
+        <v/>
+      </c>
+      <c r="P22">
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,P6,                activity_month,P4,                region,$B22)</f>
+        <v/>
+      </c>
+      <c r="Q22">
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,Q6,                activity_month,Q4,                region,$B22)</f>
+        <v/>
+      </c>
+      <c r="R22">
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,R6,                activity_month,R4,                region,$B22)</f>
+        <v/>
+      </c>
+      <c r="S22">
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,S6,                activity_month,S4,                region,$B22)</f>
+        <v/>
+      </c>
+      <c r="T22">
+        <f>SUMIFS(                INDIRECT($A22),                activity_year,T6,                activity_month,T4,                region,$B22)</f>
         <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>wtd_mfn_net_ord_gms</t>
+          <t>wtd_threep_net_ord_units</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Emerging</t>
-        </is>
-      </c>
-      <c r="J23">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,J4,activity_week,J3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="K23">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,K4,activity_week,K3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="L23">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,L4,activity_week,L3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="M23">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,M4,activity_week,M3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="N23">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,N4,activity_week,N3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="O23">
-        <f>SUMIFS(wtd_mfn_net_ord_gms,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+          <t>AGG</t>
+        </is>
+      </c>
+      <c r="I23" s="5" t="inlineStr">
+        <is>
+          <t>Net Ordered Units</t>
+        </is>
+      </c>
+      <c r="J23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,J6,                activity_week,J3,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="K23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,K6,                activity_week,K3,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="L23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,L6,                activity_week,L3,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="M23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,M6,                activity_week,M3,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="N23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,N6,                activity_week,N3,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="O23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,O6,                activity_week,O3,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="P23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,P6,                activity_month,P4,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="Q23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,Q6,                activity_month,Q4,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="R23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,R6,                activity_month,R4,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="S23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,S6,                activity_month,S4,                region,$B23)</f>
+        <v/>
+      </c>
+      <c r="T23" s="6">
+        <f>SUMIFS(                INDIRECT($A23),                activity_year,T6,                activity_month,T4,                region,$B23)</f>
         <v/>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>wtd_mfn_net_ord_units</t>
+          <t>wtd_threep_net_ord_units</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1038,35 +1615,60 @@
           <t>NA</t>
         </is>
       </c>
+      <c r="I24" s="7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="J24">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,J6,                activity_week,J3,                region,$B24)</f>
         <v/>
       </c>
       <c r="K24">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,K6,                activity_week,K3,                region,$B24)</f>
         <v/>
       </c>
       <c r="L24">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,L6,                activity_week,L3,                region,$B24)</f>
         <v/>
       </c>
       <c r="M24">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,M6,                activity_week,M3,                region,$B24)</f>
         <v/>
       </c>
       <c r="N24">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,N6,                activity_week,N3,                region,$B24)</f>
         <v/>
       </c>
       <c r="O24">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,O6,                activity_week,O3,                region,$B24)</f>
+        <v/>
+      </c>
+      <c r="P24">
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,P6,                activity_month,P4,                region,$B24)</f>
+        <v/>
+      </c>
+      <c r="Q24">
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,Q6,                activity_month,Q4,                region,$B24)</f>
+        <v/>
+      </c>
+      <c r="R24">
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,R6,                activity_month,R4,                region,$B24)</f>
+        <v/>
+      </c>
+      <c r="S24">
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,S6,                activity_month,S4,                region,$B24)</f>
+        <v/>
+      </c>
+      <c r="T24">
+        <f>SUMIFS(                INDIRECT($A24),                activity_year,T6,                activity_month,T4,                region,$B24)</f>
         <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>wtd_mfn_net_ord_units</t>
+          <t>wtd_threep_net_ord_units</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1074,35 +1676,60 @@
           <t>EU</t>
         </is>
       </c>
+      <c r="I25" s="7" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
       <c r="J25">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,J6,                activity_week,J3,                region,$B25)</f>
         <v/>
       </c>
       <c r="K25">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,K6,                activity_week,K3,                region,$B25)</f>
         <v/>
       </c>
       <c r="L25">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,L6,                activity_week,L3,                region,$B25)</f>
         <v/>
       </c>
       <c r="M25">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,M6,                activity_week,M3,                region,$B25)</f>
         <v/>
       </c>
       <c r="N25">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,N6,                activity_week,N3,                region,$B25)</f>
         <v/>
       </c>
       <c r="O25">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,O6,                activity_week,O3,                region,$B25)</f>
+        <v/>
+      </c>
+      <c r="P25">
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,P6,                activity_month,P4,                region,$B25)</f>
+        <v/>
+      </c>
+      <c r="Q25">
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,Q6,                activity_month,Q4,                region,$B25)</f>
+        <v/>
+      </c>
+      <c r="R25">
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,R6,                activity_month,R4,                region,$B25)</f>
+        <v/>
+      </c>
+      <c r="S25">
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,S6,                activity_month,S4,                region,$B25)</f>
+        <v/>
+      </c>
+      <c r="T25">
+        <f>SUMIFS(                INDIRECT($A25),                activity_year,T6,                activity_month,T4,                region,$B25)</f>
         <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>wtd_mfn_net_ord_units</t>
+          <t>wtd_threep_net_ord_units</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1110,71 +1737,121 @@
           <t>JP</t>
         </is>
       </c>
+      <c r="I26" s="7" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="J26">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,J6,                activity_week,J3,                region,$B26)</f>
         <v/>
       </c>
       <c r="K26">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,K6,                activity_week,K3,                region,$B26)</f>
         <v/>
       </c>
       <c r="L26">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,L6,                activity_week,L3,                region,$B26)</f>
         <v/>
       </c>
       <c r="M26">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,M6,                activity_week,M3,                region,$B26)</f>
         <v/>
       </c>
       <c r="N26">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,N6,                activity_week,N3,                region,$B26)</f>
         <v/>
       </c>
       <c r="O26">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,O6,                activity_week,O3,                region,$B26)</f>
+        <v/>
+      </c>
+      <c r="P26">
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,P6,                activity_month,P4,                region,$B26)</f>
+        <v/>
+      </c>
+      <c r="Q26">
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,Q6,                activity_month,Q4,                region,$B26)</f>
+        <v/>
+      </c>
+      <c r="R26">
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,R6,                activity_month,R4,                region,$B26)</f>
+        <v/>
+      </c>
+      <c r="S26">
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,S6,                activity_month,S4,                region,$B26)</f>
+        <v/>
+      </c>
+      <c r="T26">
+        <f>SUMIFS(                INDIRECT($A26),                activity_year,T6,                activity_month,T4,                region,$B26)</f>
         <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>wtd_mfn_net_ord_units</t>
+          <t>wtd_fba_net_ord_units</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Emerging</t>
-        </is>
-      </c>
-      <c r="J27">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,J4,activity_week,J3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="K27">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,K4,activity_week,K3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="L27">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,L4,activity_week,L3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="M27">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,M4,activity_week,M3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="N27">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,N4,activity_week,N3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="O27">
-        <f>SUMIFS(wtd_mfn_net_ord_units,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+          <t>AGG</t>
+        </is>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
+          <t>FBA Net Ordered Units</t>
+        </is>
+      </c>
+      <c r="J27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,J6,                activity_week,J3,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="K27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,K6,                activity_week,K3,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="L27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,L6,                activity_week,L3,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="M27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,M6,                activity_week,M3,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="N27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,N6,                activity_week,N3,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="O27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,O6,                activity_week,O3,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="P27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,P6,                activity_month,P4,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="Q27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,Q6,                activity_month,Q4,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="R27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,R6,                activity_month,R4,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="S27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,S6,                activity_month,S4,                region,$B27)</f>
+        <v/>
+      </c>
+      <c r="T27" s="6">
+        <f>SUMIFS(                INDIRECT($A27),                activity_year,T6,                activity_month,T4,                region,$B27)</f>
         <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>wtd_net_ord_gms</t>
+          <t>wtd_fba_net_ord_units</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1182,35 +1859,60 @@
           <t>NA</t>
         </is>
       </c>
+      <c r="I28" s="7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="J28">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,J6,                activity_week,J3,                region,$B28)</f>
         <v/>
       </c>
       <c r="K28">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,K6,                activity_week,K3,                region,$B28)</f>
         <v/>
       </c>
       <c r="L28">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,L6,                activity_week,L3,                region,$B28)</f>
         <v/>
       </c>
       <c r="M28">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,M6,                activity_week,M3,                region,$B28)</f>
         <v/>
       </c>
       <c r="N28">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,N6,                activity_week,N3,                region,$B28)</f>
         <v/>
       </c>
       <c r="O28">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,O6,                activity_week,O3,                region,$B28)</f>
+        <v/>
+      </c>
+      <c r="P28">
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,P6,                activity_month,P4,                region,$B28)</f>
+        <v/>
+      </c>
+      <c r="Q28">
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,Q6,                activity_month,Q4,                region,$B28)</f>
+        <v/>
+      </c>
+      <c r="R28">
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,R6,                activity_month,R4,                region,$B28)</f>
+        <v/>
+      </c>
+      <c r="S28">
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,S6,                activity_month,S4,                region,$B28)</f>
+        <v/>
+      </c>
+      <c r="T28">
+        <f>SUMIFS(                INDIRECT($A28),                activity_year,T6,                activity_month,T4,                region,$B28)</f>
         <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>wtd_net_ord_gms</t>
+          <t>wtd_fba_net_ord_units</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1218,35 +1920,60 @@
           <t>EU</t>
         </is>
       </c>
+      <c r="I29" s="7" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
       <c r="J29">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,J6,                activity_week,J3,                region,$B29)</f>
         <v/>
       </c>
       <c r="K29">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,K6,                activity_week,K3,                region,$B29)</f>
         <v/>
       </c>
       <c r="L29">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,L6,                activity_week,L3,                region,$B29)</f>
         <v/>
       </c>
       <c r="M29">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,M6,                activity_week,M3,                region,$B29)</f>
         <v/>
       </c>
       <c r="N29">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,N6,                activity_week,N3,                region,$B29)</f>
         <v/>
       </c>
       <c r="O29">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,O6,                activity_week,O3,                region,$B29)</f>
+        <v/>
+      </c>
+      <c r="P29">
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,P6,                activity_month,P4,                region,$B29)</f>
+        <v/>
+      </c>
+      <c r="Q29">
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,Q6,                activity_month,Q4,                region,$B29)</f>
+        <v/>
+      </c>
+      <c r="R29">
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,R6,                activity_month,R4,                region,$B29)</f>
+        <v/>
+      </c>
+      <c r="S29">
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,S6,                activity_month,S4,                region,$B29)</f>
+        <v/>
+      </c>
+      <c r="T29">
+        <f>SUMIFS(                INDIRECT($A29),                activity_year,T6,                activity_month,T4,                region,$B29)</f>
         <v/>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>wtd_net_ord_gms</t>
+          <t>wtd_fba_net_ord_units</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1254,71 +1981,121 @@
           <t>JP</t>
         </is>
       </c>
+      <c r="I30" s="7" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="J30">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,J6,                activity_week,J3,                region,$B30)</f>
         <v/>
       </c>
       <c r="K30">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,K6,                activity_week,K3,                region,$B30)</f>
         <v/>
       </c>
       <c r="L30">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,L6,                activity_week,L3,                region,$B30)</f>
         <v/>
       </c>
       <c r="M30">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,M6,                activity_week,M3,                region,$B30)</f>
         <v/>
       </c>
       <c r="N30">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,N6,                activity_week,N3,                region,$B30)</f>
         <v/>
       </c>
       <c r="O30">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,O4,activity_week,O3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,O6,                activity_week,O3,                region,$B30)</f>
+        <v/>
+      </c>
+      <c r="P30">
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,P6,                activity_month,P4,                region,$B30)</f>
+        <v/>
+      </c>
+      <c r="Q30">
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,Q6,                activity_month,Q4,                region,$B30)</f>
+        <v/>
+      </c>
+      <c r="R30">
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,R6,                activity_month,R4,                region,$B30)</f>
+        <v/>
+      </c>
+      <c r="S30">
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,S6,                activity_month,S4,                region,$B30)</f>
+        <v/>
+      </c>
+      <c r="T30">
+        <f>SUMIFS(                INDIRECT($A30),                activity_year,T6,                activity_month,T4,                region,$B30)</f>
         <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>wtd_net_ord_gms</t>
+          <t>wtd_mfn_net_ord_units</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Emerging</t>
-        </is>
-      </c>
-      <c r="J31">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,J4,activity_week,J3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="K31">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,K4,activity_week,K3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="L31">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,L4,activity_week,L3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="M31">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,M4,activity_week,M3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="N31">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,N4,activity_week,N3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="O31">
-        <f>SUMIFS(wtd_net_ord_gms,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+          <t>AGG</t>
+        </is>
+      </c>
+      <c r="I31" s="5" t="inlineStr">
+        <is>
+          <t>MFN Net Ordered Units</t>
+        </is>
+      </c>
+      <c r="J31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,J6,                activity_week,J3,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="K31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,K6,                activity_week,K3,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="L31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,L6,                activity_week,L3,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="M31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,M6,                activity_week,M3,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="N31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,N6,                activity_week,N3,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="O31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,O6,                activity_week,O3,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="P31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,P6,                activity_month,P4,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="Q31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,Q6,                activity_month,Q4,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="R31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,R6,                activity_month,R4,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="S31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,S6,                activity_month,S4,                region,$B31)</f>
+        <v/>
+      </c>
+      <c r="T31" s="6">
+        <f>SUMIFS(                INDIRECT($A31),                activity_year,T6,                activity_month,T4,                region,$B31)</f>
         <v/>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>wtd_net_ord_units</t>
+          <t>wtd_mfn_net_ord_units</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1326,35 +2103,60 @@
           <t>NA</t>
         </is>
       </c>
+      <c r="I32" s="7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="J32">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,J4,activity_week,J3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,J6,                activity_week,J3,                region,$B32)</f>
         <v/>
       </c>
       <c r="K32">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,K4,activity_week,K3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,K6,                activity_week,K3,                region,$B32)</f>
         <v/>
       </c>
       <c r="L32">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,L4,activity_week,L3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,L6,                activity_week,L3,                region,$B32)</f>
         <v/>
       </c>
       <c r="M32">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,M4,activity_week,M3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,M6,                activity_week,M3,                region,$B32)</f>
         <v/>
       </c>
       <c r="N32">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,N4,activity_week,N3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,N6,                activity_week,N3,                region,$B32)</f>
         <v/>
       </c>
       <c r="O32">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,O4,activity_week,O3,region,"NA")</f>
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,O6,                activity_week,O3,                region,$B32)</f>
+        <v/>
+      </c>
+      <c r="P32">
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,P6,                activity_month,P4,                region,$B32)</f>
+        <v/>
+      </c>
+      <c r="Q32">
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,Q6,                activity_month,Q4,                region,$B32)</f>
+        <v/>
+      </c>
+      <c r="R32">
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,R6,                activity_month,R4,                region,$B32)</f>
+        <v/>
+      </c>
+      <c r="S32">
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,S6,                activity_month,S4,                region,$B32)</f>
+        <v/>
+      </c>
+      <c r="T32">
+        <f>SUMIFS(                INDIRECT($A32),                activity_year,T6,                activity_month,T4,                region,$B32)</f>
         <v/>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>wtd_net_ord_units</t>
+          <t>wtd_mfn_net_ord_units</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1362,35 +2164,60 @@
           <t>EU</t>
         </is>
       </c>
+      <c r="I33" s="7" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
       <c r="J33">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,J4,activity_week,J3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,J6,                activity_week,J3,                region,$B33)</f>
         <v/>
       </c>
       <c r="K33">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,K4,activity_week,K3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,K6,                activity_week,K3,                region,$B33)</f>
         <v/>
       </c>
       <c r="L33">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,L4,activity_week,L3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,L6,                activity_week,L3,                region,$B33)</f>
         <v/>
       </c>
       <c r="M33">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,M4,activity_week,M3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,M6,                activity_week,M3,                region,$B33)</f>
         <v/>
       </c>
       <c r="N33">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,N4,activity_week,N3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,N6,                activity_week,N3,                region,$B33)</f>
         <v/>
       </c>
       <c r="O33">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,O4,activity_week,O3,region,"EU")</f>
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,O6,                activity_week,O3,                region,$B33)</f>
+        <v/>
+      </c>
+      <c r="P33">
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,P6,                activity_month,P4,                region,$B33)</f>
+        <v/>
+      </c>
+      <c r="Q33">
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,Q6,                activity_month,Q4,                region,$B33)</f>
+        <v/>
+      </c>
+      <c r="R33">
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,R6,                activity_month,R4,                region,$B33)</f>
+        <v/>
+      </c>
+      <c r="S33">
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,S6,                activity_month,S4,                region,$B33)</f>
+        <v/>
+      </c>
+      <c r="T33">
+        <f>SUMIFS(                INDIRECT($A33),                activity_year,T6,                activity_month,T4,                region,$B33)</f>
         <v/>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>wtd_net_ord_units</t>
+          <t>wtd_mfn_net_ord_units</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1398,64 +2225,53 @@
           <t>JP</t>
         </is>
       </c>
+      <c r="I34" s="7" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="J34">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,J4,activity_week,J3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,J6,                activity_week,J3,                region,$B34)</f>
         <v/>
       </c>
       <c r="K34">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,K4,activity_week,K3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,K6,                activity_week,K3,                region,$B34)</f>
         <v/>
       </c>
       <c r="L34">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,L4,activity_week,L3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,L6,                activity_week,L3,                region,$B34)</f>
         <v/>
       </c>
       <c r="M34">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,M4,activity_week,M3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,M6,                activity_week,M3,                region,$B34)</f>
         <v/>
       </c>
       <c r="N34">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,N4,activity_week,N3,region,"JP")</f>
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,N6,                activity_week,N3,                region,$B34)</f>
         <v/>
       </c>
       <c r="O34">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,O4,activity_week,O3,region,"JP")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>wtd_net_ord_units</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Emerging</t>
-        </is>
-      </c>
-      <c r="J35">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,J4,activity_week,J3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="K35">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,K4,activity_week,K3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="L35">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,L4,activity_week,L3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="M35">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,M4,activity_week,M3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="N35">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,N4,activity_week,N3,region,"Emerging")</f>
-        <v/>
-      </c>
-      <c r="O35">
-        <f>SUMIFS(wtd_net_ord_units,activity_year,O4,activity_week,O3,region,"Emerging")</f>
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,O6,                activity_week,O3,                region,$B34)</f>
+        <v/>
+      </c>
+      <c r="P34">
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,P6,                activity_month,P4,                region,$B34)</f>
+        <v/>
+      </c>
+      <c r="Q34">
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,Q6,                activity_month,Q4,                region,$B34)</f>
+        <v/>
+      </c>
+      <c r="R34">
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,R6,                activity_month,R4,                region,$B34)</f>
+        <v/>
+      </c>
+      <c r="S34">
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,S6,                activity_month,S4,                region,$B34)</f>
+        <v/>
+      </c>
+      <c r="T34">
+        <f>SUMIFS(                INDIRECT($A34),                activity_year,T6,                activity_month,T4,                region,$B34)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
add the time series layout
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,24 +423,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SELLER ORIGIN</t>
+        </is>
+      </c>
+      <c r="B1">
         <f>__METADATA__!B3</f>
         <v/>
       </c>
       <c r="J1" t="n">
-        <v>-6</v>
+        <v>-28</v>
       </c>
       <c r="K1" t="n">
-        <v>-5</v>
+        <v>-21</v>
       </c>
       <c r="L1" t="n">
-        <v>-4</v>
+        <v>-14</v>
       </c>
       <c r="M1" t="n">
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="N1" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="O1" t="n">
         <v>-4</v>
@@ -449,70 +454,159 @@
         <v>-3</v>
       </c>
       <c r="Q1" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="R1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S1" t="n">
         <v>-2</v>
       </c>
+      <c r="T1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="B2">
         <f>__METADATA__!B1</f>
         <v/>
       </c>
       <c r="J2">
-        <f>A2 + 0</f>
+        <f>B2 + J1</f>
         <v/>
       </c>
       <c r="K2">
-        <f>A2 + 1</f>
+        <f>B2 + K1</f>
         <v/>
       </c>
       <c r="L2">
-        <f>A2 + 2</f>
+        <f>B2 + L1</f>
         <v/>
       </c>
       <c r="M2">
-        <f>A2 + 3</f>
+        <f>B2 + M1</f>
         <v/>
       </c>
       <c r="N2">
-        <f>EOMONTH(A2, 0)</f>
+        <f>B2 + N1</f>
         <v/>
       </c>
       <c r="O2">
-        <f>EOMONTH(A2, 1)</f>
+        <f>EOMONTH(B2, O1)</f>
         <v/>
       </c>
       <c r="P2">
-        <f>EOMONTH(A2, 2)</f>
+        <f>EOMONTH(B2, P1)</f>
         <v/>
       </c>
       <c r="Q2">
-        <f>EOMONTH(A2, 0)</f>
+        <f>EOMONTH(B2, Q1)</f>
         <v/>
       </c>
       <c r="R2">
-        <f>A2 + 0</f>
+        <f>EOMONTH(B2, R1)</f>
+        <v/>
+      </c>
+      <c r="S2">
+        <f>EOMONTH(B2, S1)</f>
+        <v/>
+      </c>
+      <c r="T2">
+        <f>EOMONTH(B2, T1)</f>
+        <v/>
+      </c>
+      <c r="U2">
+        <f>B2 + U1</f>
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>REGION</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>ALL</t>
         </is>
+      </c>
+      <c r="J3">
+        <f>_xlfn.ISOWEEKNUM(J2 + 1)</f>
+        <v/>
+      </c>
+      <c r="K3">
+        <f>_xlfn.ISOWEEKNUM(K2 + 1)</f>
+        <v/>
+      </c>
+      <c r="L3">
+        <f>_xlfn.ISOWEEKNUM(L2 + 1)</f>
+        <v/>
+      </c>
+      <c r="M3">
+        <f>_xlfn.ISOWEEKNUM(M2 + 1)</f>
+        <v/>
+      </c>
+      <c r="N3">
+        <f>_xlfn.ISOWEEKNUM(N2 + 1)</f>
+        <v/>
+      </c>
+      <c r="O3">
+        <f>MONTH(O2)</f>
+        <v/>
+      </c>
+      <c r="P3">
+        <f>MONTH(P2)</f>
+        <v/>
+      </c>
+      <c r="Q3">
+        <f>MONTH(Q2)</f>
+        <v/>
+      </c>
+      <c r="R3">
+        <f>MONTH(R2)</f>
+        <v/>
+      </c>
+      <c r="S3">
+        <f>_xlfn.ROUNDUP(MONTH(S2)/3,0)</f>
+        <v/>
+      </c>
+      <c r="T3">
+        <f>_xlfn.ROUNDUP(MONTH(T2)/3,0)</f>
+        <v/>
+      </c>
+      <c r="U3">
+        <f>_xlfn.ISOWEEKNUM(U2 + 1)</f>
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>MARKETPLACE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
+        <is>
+          <t>TEAM</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>ALL</t>
         </is>

</xml_diff>